<commit_message>
changing for shiny app
</commit_message>
<xml_diff>
--- a/COVIDPPP/bankbybank.xlsx
+++ b/COVIDPPP/bankbybank.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Justin\Gov50\pppdata\COVIDPPP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8AD749D-99D4-483D-8327-EBFC96780381}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C48489-EA3B-4741-8F01-687DB124D35E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="-1840" windowWidth="19420" windowHeight="10420" xr2:uid="{8E8865FE-907F-F142-8AE8-1C4958F5B415}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="98">
   <si>
     <t>BofA</t>
   </si>
@@ -61,24 +61,12 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>0.003</t>
-  </si>
-  <si>
-    <t>0.007</t>
-  </si>
-  <si>
-    <t>(0.043)</t>
-  </si>
-  <si>
     <t>(0.045)</t>
   </si>
   <si>
     <t>(0.044)</t>
   </si>
   <si>
-    <t>(0.042)</t>
-  </si>
-  <si>
     <t>(0.019)</t>
   </si>
   <si>
@@ -88,9 +76,6 @@
     <t>(0.017)</t>
   </si>
   <si>
-    <t>(0.119)</t>
-  </si>
-  <si>
     <t>R2</t>
   </si>
   <si>
@@ -106,9 +91,6 @@
     <t>(0.003)</t>
   </si>
   <si>
-    <t>(0.006)</t>
-  </si>
-  <si>
     <t>(0.002)</t>
   </si>
   <si>
@@ -121,84 +103,18 @@
     <t>National</t>
   </si>
   <si>
-    <t>0.027***</t>
-  </si>
-  <si>
-    <t>0.023***</t>
-  </si>
-  <si>
-    <t>0.022***</t>
-  </si>
-  <si>
-    <t>0.033***</t>
-  </si>
-  <si>
-    <t>0.024***</t>
-  </si>
-  <si>
-    <t>-1.705***</t>
-  </si>
-  <si>
-    <t>0.253</t>
-  </si>
-  <si>
-    <t>0.059</t>
-  </si>
-  <si>
-    <t>1.331***</t>
-  </si>
-  <si>
-    <t>-0.415***</t>
-  </si>
-  <si>
-    <t>2.109***</t>
-  </si>
-  <si>
-    <t>(0.246)</t>
-  </si>
-  <si>
     <t>(0.100)</t>
   </si>
   <si>
-    <t>(0.088)</t>
-  </si>
-  <si>
-    <t>(0.081)</t>
-  </si>
-  <si>
-    <t>(0.095)</t>
-  </si>
-  <si>
-    <t>-0.026***</t>
-  </si>
-  <si>
-    <t>-0.037***</t>
-  </si>
-  <si>
     <t>0.002</t>
   </si>
   <si>
-    <t>-0.002</t>
-  </si>
-  <si>
-    <t>-0.024***</t>
-  </si>
-  <si>
     <t>-0.032***</t>
   </si>
   <si>
-    <t>0.812</t>
-  </si>
-  <si>
-    <t>0.811</t>
-  </si>
-  <si>
     <t xml:space="preserve">Adj. R2 </t>
   </si>
   <si>
-    <t>0.810</t>
-  </si>
-  <si>
     <t>Num. groups: fips</t>
   </si>
   <si>
@@ -208,48 +124,6 @@
     <t>Credit Union</t>
   </si>
   <si>
-    <t>-1.255</t>
-  </si>
-  <si>
-    <t>2.451*</t>
-  </si>
-  <si>
-    <t>-3.597***</t>
-  </si>
-  <si>
-    <t>1.046</t>
-  </si>
-  <si>
-    <t>-0.684</t>
-  </si>
-  <si>
-    <t>3.096***</t>
-  </si>
-  <si>
-    <t>(0.929)</t>
-  </si>
-  <si>
-    <t>(1.223)</t>
-  </si>
-  <si>
-    <t>(0.835)</t>
-  </si>
-  <si>
-    <t>(0.749)</t>
-  </si>
-  <si>
-    <t>(0.422)</t>
-  </si>
-  <si>
-    <t>(0.577)</t>
-  </si>
-  <si>
-    <t>-0.058*</t>
-  </si>
-  <si>
-    <t>-0.068</t>
-  </si>
-  <si>
     <t>0.073**</t>
   </si>
   <si>
@@ -259,28 +133,193 @@
     <t>-0.040*</t>
   </si>
   <si>
-    <t>-0.025</t>
-  </si>
-  <si>
     <t>(0.026)</t>
   </si>
   <si>
-    <t>(0.036)</t>
-  </si>
-  <si>
-    <t>0.012</t>
-  </si>
-  <si>
-    <t>-0.005</t>
-  </si>
-  <si>
     <t>0.000</t>
   </si>
   <si>
-    <t>0.015</t>
-  </si>
-  <si>
     <t xml:space="preserve">R2 </t>
+  </si>
+  <si>
+    <t>0.036***</t>
+  </si>
+  <si>
+    <t>0.030***</t>
+  </si>
+  <si>
+    <t>0.029***</t>
+  </si>
+  <si>
+    <t>0.047***</t>
+  </si>
+  <si>
+    <t>0.031***</t>
+  </si>
+  <si>
+    <t>(0.004)</t>
+  </si>
+  <si>
+    <t>-1.542***</t>
+  </si>
+  <si>
+    <t>0.298</t>
+  </si>
+  <si>
+    <t>-0.206</t>
+  </si>
+  <si>
+    <t>1.288***</t>
+  </si>
+  <si>
+    <t>-0.302**</t>
+  </si>
+  <si>
+    <t>2.474***</t>
+  </si>
+  <si>
+    <t>(0.146)</t>
+  </si>
+  <si>
+    <t>(0.155)</t>
+  </si>
+  <si>
+    <t>(0.118)</t>
+  </si>
+  <si>
+    <t>(0.103)</t>
+  </si>
+  <si>
+    <t>(0.092)</t>
+  </si>
+  <si>
+    <t>-0.036***</t>
+  </si>
+  <si>
+    <t>-0.047***</t>
+  </si>
+  <si>
+    <t>0.001</t>
+  </si>
+  <si>
+    <t>-0.040***</t>
+  </si>
+  <si>
+    <t>0.753</t>
+  </si>
+  <si>
+    <t>0.751</t>
+  </si>
+  <si>
+    <t>0.752</t>
+  </si>
+  <si>
+    <t>(Intercept)</t>
+  </si>
+  <si>
+    <t>39.375</t>
+  </si>
+  <si>
+    <t>39.852</t>
+  </si>
+  <si>
+    <t>40.503</t>
+  </si>
+  <si>
+    <t>40.620</t>
+  </si>
+  <si>
+    <t>38.826</t>
+  </si>
+  <si>
+    <t>41.183</t>
+  </si>
+  <si>
+    <t>(20.820)</t>
+  </si>
+  <si>
+    <t>(21.011)</t>
+  </si>
+  <si>
+    <t>(20.991)</t>
+  </si>
+  <si>
+    <t>(21.007)</t>
+  </si>
+  <si>
+    <t>(20.930)</t>
+  </si>
+  <si>
+    <t>(21.129)</t>
+  </si>
+  <si>
+    <t>0.010</t>
+  </si>
+  <si>
+    <t>-0.006</t>
+  </si>
+  <si>
+    <t>-0.001</t>
+  </si>
+  <si>
+    <t>0.014</t>
+  </si>
+  <si>
+    <t>0.006</t>
+  </si>
+  <si>
+    <t>(0.046)</t>
+  </si>
+  <si>
+    <t>(0.047)</t>
+  </si>
+  <si>
+    <t>-1.292</t>
+  </si>
+  <si>
+    <t>2.122</t>
+  </si>
+  <si>
+    <t>-3.609***</t>
+  </si>
+  <si>
+    <t>1.018</t>
+  </si>
+  <si>
+    <t>-0.696</t>
+  </si>
+  <si>
+    <t>3.088***</t>
+  </si>
+  <si>
+    <t>(0.941)</t>
+  </si>
+  <si>
+    <t>(1.279)</t>
+  </si>
+  <si>
+    <t>(0.834)</t>
+  </si>
+  <si>
+    <t>(0.746)</t>
+  </si>
+  <si>
+    <t>(0.420)</t>
+  </si>
+  <si>
+    <t>(0.575)</t>
+  </si>
+  <si>
+    <t>-0.057*</t>
+  </si>
+  <si>
+    <t>-0.063</t>
+  </si>
+  <si>
+    <t>-0.026</t>
+  </si>
+  <si>
+    <t>(0.037)</t>
   </si>
 </sst>
 </file>
@@ -633,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF8A916E-8524-4D4E-9CBA-5515E1C80839}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -646,7 +685,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -669,25 +708,25 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -695,45 +734,45 @@
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>71</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -741,45 +780,45 @@
         <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>66</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>68</v>
+        <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -787,91 +826,137 @@
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>17</v>
+        <v>91</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>19</v>
+        <v>92</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>18</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>94</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>24</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>84</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>22</v>
+        <v>97</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -884,7 +969,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -894,7 +979,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -909,10 +994,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -920,22 +1005,22 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -943,22 +1028,22 @@
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -966,22 +1051,22 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -989,22 +1074,22 @@
         <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1012,22 +1097,22 @@
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1035,22 +1120,22 @@
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1058,91 +1143,91 @@
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>